<commit_message>
UserRegion with Different Users - Part 2
</commit_message>
<xml_diff>
--- a/Lexis-GLOBAL/Coredata/USER_REGION.xlsx
+++ b/Lexis-GLOBAL/Coredata/USER_REGION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adapp\git\AutoAPI\Lexis-GLOBAL\Coredata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F655C18-094D-477C-81D4-9D82AEAE7D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EA3100-B3E2-4326-A39B-620E437D82D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserRegion_View" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="71">
   <si>
     <t>S.No</t>
   </si>
@@ -1182,7 +1182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546274F2-5181-4A4E-AD1A-2405E6D1286C}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="S2" sqref="S2:S6"/>
     </sheetView>
   </sheetViews>
@@ -1633,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E310E616-82EC-4CC4-9720-1C0AE01E87DA}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1800,14 +1800,30 @@
       <c r="H3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+      <c r="I3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="Q3" s="1" t="s">
         <v>38</v>
       </c>
@@ -1815,7 +1831,7 @@
         <v>39</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="T3" s="6"/>
     </row>
@@ -1844,14 +1860,30 @@
       <c r="H4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
+      <c r="I4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="Q4" s="1" t="s">
         <v>40</v>
       </c>
@@ -1859,7 +1891,7 @@
         <v>41</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="T4" s="6"/>
     </row>
@@ -1888,14 +1920,30 @@
       <c r="H5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
+      <c r="I5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="Q5" s="1" t="s">
         <v>42</v>
       </c>
@@ -1903,7 +1951,7 @@
         <v>43</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="T5" s="6"/>
     </row>
@@ -1932,14 +1980,30 @@
       <c r="H6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
+      <c r="I6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="Q6" s="1" t="s">
         <v>44</v>
       </c>
@@ -1947,7 +2011,7 @@
         <v>45</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="T6" s="6"/>
     </row>
@@ -1976,14 +2040,30 @@
       <c r="H7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
+      <c r="I7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="Q7" s="1" t="s">
         <v>46</v>
       </c>
@@ -1991,7 +2071,7 @@
         <v>47</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="T7" s="6"/>
     </row>

</xml_diff>

<commit_message>
UserRegion with Deifferent Users Validation Final
</commit_message>
<xml_diff>
--- a/Lexis-GLOBAL/Coredata/USER_REGION.xlsx
+++ b/Lexis-GLOBAL/Coredata/USER_REGION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adapp\git\AutoAPI\Lexis-GLOBAL\Coredata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4890B4-7729-4F57-80B9-0A1C992E177F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE146A10-25C3-4F58-9113-FCF4F7D2D313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserRegion_View" sheetId="7" r:id="rId1"/>
@@ -726,7 +726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F5320C-FCCA-46FE-B3EE-3234201A0A0A}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
@@ -1179,7 +1179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546274F2-5181-4A4E-AD1A-2405E6D1286C}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="S3" sqref="S3:S7"/>
     </sheetView>
   </sheetViews>
@@ -2081,8 +2081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1FCFD6D-A0BF-4B39-BA3B-974FC5434548}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>